<commit_message>
updated orange file + xlsx files for cumulative results and optimal points for VER
</commit_message>
<xml_diff>
--- a/Historical_Cumulative_Result_test.xlsx
+++ b/Historical_Cumulative_Result_test.xlsx
@@ -113,7 +113,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -123,6 +123,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -249,10 +253,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26:A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -701,7 +705,7 @@
       <c r="A23" s="2" t="n">
         <v>45948</v>
       </c>
-      <c r="B23" s="0" t="n">
+      <c r="B23" s="1" t="n">
         <v>336</v>
       </c>
       <c r="C23" s="1" t="n">
@@ -756,6 +760,24 @@
       <c r="F25" s="1" t="n">
         <v>212</v>
       </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="3"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="3"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="3"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>